<commit_message>
Added descriptions in file Pi_Chart_regions_results_all
</commit_message>
<xml_diff>
--- a/Data/MaTraceCopper_Indata.xlsx
+++ b/Data/MaTraceCopper_Indata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9564" windowHeight="6936" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9564" windowHeight="6936"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario_Overview" sheetId="1" r:id="rId1"/>
@@ -2424,8 +2424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AI72"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2565,7 +2565,7 @@
         <v>22</v>
       </c>
       <c r="C4" s="107">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="79"/>
       <c r="F4"/>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="C6" s="6" t="str">
         <f ca="1">LOOKUP($C$4,$G$4:$G$111,$H$4:$H$114)</f>
-        <v>BAU</v>
+        <v>REUmod</v>
       </c>
       <c r="E6" s="79"/>
       <c r="G6" s="3">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="C7" s="6" t="str">
         <f ca="1">LOOKUP($C$4,$G$4:$G$111,$I$4:$I$114)</f>
-        <v>BAU</v>
+        <v>(1a) increase reuse moderate</v>
       </c>
       <c r="E7" s="79"/>
       <c r="G7" s="3">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="C19" s="6" t="str">
         <f ca="1">LOOKUP($C$4,$G$4:$G$112,$S$4:$S$66)</f>
-        <v>no</v>
+        <v>Moderate</v>
       </c>
       <c r="E19" s="79"/>
       <c r="G19" s="3">
@@ -3924,9 +3924,9 @@
       <c r="B24" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="6" t="str">
         <f ca="1">LOOKUP($C$4,$G$4:$G$112,$Y$4:$Y$66)</f>
-        <v>0</v>
+        <v>Basic</v>
       </c>
       <c r="E24" s="79"/>
       <c r="G24" s="3">
@@ -5965,8 +5965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39102,7 +39102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>

</xml_diff>